<commit_message>
Commit Spring and Dampers
</commit_message>
<xml_diff>
--- a/mbs-EP-v.1.0.0/Excel Files/crank_slider.xlsx
+++ b/mbs-EP-v.1.0.0/Excel Files/crank_slider.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago_Serralha\Desktop\Thesis-Project\mbs-EP-v.1.0.0\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9D75CD9-7606-4158-902D-3235F8D74FAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD0DA655-252E-414F-BD73-A196548C26EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SimParam" sheetId="4" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="251">
   <si>
     <t>Mass</t>
   </si>
@@ -838,6 +838,9 @@
   </si>
   <si>
     <t>Important Note</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -1286,6 +1289,51 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1323,41 +1371,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1385,71 +1403,59 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1479,9 +1485,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1929,8 +1932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE954C49-6E73-4D49-8054-42AF7A10140C}">
   <dimension ref="B2:Q39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:Q2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1949,44 +1952,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B2" s="83" t="s">
+      <c r="B2" s="70" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="85"/>
-      <c r="J2" s="82" t="s">
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="72"/>
+      <c r="J2" s="66" t="s">
         <v>166</v>
       </c>
-      <c r="K2" s="82"/>
-      <c r="L2" s="82"/>
-      <c r="M2" s="82"/>
-      <c r="N2" s="82"/>
-      <c r="O2" s="82"/>
-      <c r="P2" s="82"/>
-      <c r="Q2" s="82"/>
+      <c r="K2" s="66"/>
+      <c r="L2" s="66"/>
+      <c r="M2" s="66"/>
+      <c r="N2" s="66"/>
+      <c r="O2" s="66"/>
+      <c r="P2" s="66"/>
+      <c r="Q2" s="66"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B3" s="80" t="s">
+      <c r="B3" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="81"/>
+      <c r="C3" s="69"/>
       <c r="D3" s="54">
         <v>2</v>
       </c>
       <c r="E3" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="J3" s="99" t="s">
+      <c r="J3" s="76" t="s">
         <v>115</v>
       </c>
-      <c r="K3" s="100"/>
-      <c r="L3" s="101"/>
-      <c r="M3" s="99" t="s">
+      <c r="K3" s="77"/>
+      <c r="L3" s="78"/>
+      <c r="M3" s="76" t="s">
         <v>141</v>
       </c>
-      <c r="N3" s="100"/>
-      <c r="O3" s="75"/>
+      <c r="N3" s="77"/>
+      <c r="O3" s="90"/>
       <c r="P3" s="48" t="s">
         <v>172</v>
       </c>
@@ -1995,12 +1998,12 @@
       </c>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B4" s="80" t="s">
+      <c r="B4" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="81"/>
+      <c r="C4" s="69"/>
       <c r="D4" s="54">
-        <v>0.05</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E4" s="54" t="s">
         <v>22</v>
@@ -2011,14 +2014,14 @@
       <c r="K4" s="48" t="s">
         <v>109</v>
       </c>
-      <c r="L4" s="102"/>
+      <c r="L4" s="79"/>
       <c r="M4" s="46" t="s">
         <v>142</v>
       </c>
       <c r="N4" s="48" t="s">
         <v>143</v>
       </c>
-      <c r="O4" s="76"/>
+      <c r="O4" s="91"/>
       <c r="P4" s="48" t="s">
         <v>173</v>
       </c>
@@ -2027,10 +2030,10 @@
       </c>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B5" s="80" t="s">
+      <c r="B5" s="68" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="81"/>
+      <c r="C5" s="69"/>
       <c r="D5" s="54" t="s">
         <v>91</v>
       </c>
@@ -2043,14 +2046,14 @@
       <c r="K5" s="48" t="s">
         <v>110</v>
       </c>
-      <c r="L5" s="102"/>
+      <c r="L5" s="79"/>
       <c r="M5" s="48" t="s">
         <v>5</v>
       </c>
       <c r="N5" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="O5" s="76"/>
+      <c r="O5" s="91"/>
       <c r="P5" s="48" t="s">
         <v>174</v>
       </c>
@@ -2059,10 +2062,10 @@
       </c>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B6" s="80" t="s">
+      <c r="B6" s="68" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="81"/>
+      <c r="C6" s="69"/>
       <c r="D6" s="54"/>
       <c r="E6" s="54" t="s">
         <v>88</v>
@@ -2073,14 +2076,14 @@
       <c r="K6" s="48" t="s">
         <v>111</v>
       </c>
-      <c r="L6" s="102"/>
+      <c r="L6" s="79"/>
       <c r="M6" s="48" t="s">
         <v>144</v>
       </c>
       <c r="N6" s="48" t="s">
         <v>145</v>
       </c>
-      <c r="O6" s="76"/>
+      <c r="O6" s="91"/>
       <c r="P6" s="48" t="s">
         <v>178</v>
       </c>
@@ -2089,10 +2092,10 @@
       </c>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B7" s="80" t="s">
+      <c r="B7" s="68" t="s">
         <v>89</v>
       </c>
-      <c r="C7" s="81"/>
+      <c r="C7" s="69"/>
       <c r="D7" s="54"/>
       <c r="E7" s="55" t="s">
         <v>118</v>
@@ -2103,14 +2106,14 @@
       <c r="K7" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="L7" s="102"/>
+      <c r="L7" s="79"/>
       <c r="M7" s="48" t="s">
         <v>10</v>
       </c>
       <c r="N7" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="O7" s="76"/>
+      <c r="O7" s="91"/>
       <c r="P7" s="48" t="s">
         <v>177</v>
       </c>
@@ -2119,10 +2122,10 @@
       </c>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B8" s="80" t="s">
+      <c r="B8" s="68" t="s">
         <v>96</v>
       </c>
-      <c r="C8" s="81"/>
+      <c r="C8" s="69"/>
       <c r="D8" s="54" t="s">
         <v>140</v>
       </c>
@@ -2135,14 +2138,14 @@
       <c r="K8" s="48" t="s">
         <v>114</v>
       </c>
-      <c r="L8" s="102"/>
+      <c r="L8" s="79"/>
       <c r="M8" s="48" t="s">
         <v>12</v>
       </c>
       <c r="N8" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="O8" s="76"/>
+      <c r="O8" s="91"/>
       <c r="P8" s="48" t="s">
         <v>181</v>
       </c>
@@ -2151,10 +2154,10 @@
       </c>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B9" s="80" t="s">
+      <c r="B9" s="68" t="s">
         <v>133</v>
       </c>
-      <c r="C9" s="81"/>
+      <c r="C9" s="69"/>
       <c r="D9" s="54"/>
       <c r="E9" s="55" t="s">
         <v>134</v>
@@ -2165,14 +2168,14 @@
       <c r="K9" s="48" t="s">
         <v>112</v>
       </c>
-      <c r="L9" s="102"/>
+      <c r="L9" s="79"/>
       <c r="M9" s="48" t="s">
         <v>13</v>
       </c>
       <c r="N9" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="O9" s="76"/>
+      <c r="O9" s="91"/>
       <c r="P9" s="48" t="s">
         <v>182</v>
       </c>
@@ -2187,14 +2190,14 @@
       <c r="K10" s="32" t="s">
         <v>121</v>
       </c>
-      <c r="L10" s="102"/>
+      <c r="L10" s="79"/>
       <c r="M10" s="48" t="s">
         <v>14</v>
       </c>
       <c r="N10" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="O10" s="76"/>
+      <c r="O10" s="91"/>
       <c r="P10" s="53" t="s">
         <v>183</v>
       </c>
@@ -2205,14 +2208,14 @@
     <row r="11" spans="2:17" x14ac:dyDescent="0.25">
       <c r="J11" s="57"/>
       <c r="K11" s="58"/>
-      <c r="L11" s="102"/>
+      <c r="L11" s="79"/>
       <c r="M11" s="48" t="s">
         <v>146</v>
       </c>
       <c r="N11" s="48" t="s">
         <v>146</v>
       </c>
-      <c r="O11" s="76"/>
+      <c r="O11" s="91"/>
       <c r="P11" s="53" t="s">
         <v>184</v>
       </c>
@@ -2221,25 +2224,25 @@
       </c>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B12" s="88" t="s">
+      <c r="B12" s="74" t="s">
         <v>150</v>
       </c>
-      <c r="C12" s="89"/>
-      <c r="D12" s="89"/>
-      <c r="E12" s="89"/>
-      <c r="F12" s="89"/>
-      <c r="G12" s="89"/>
-      <c r="H12" s="89"/>
+      <c r="C12" s="75"/>
+      <c r="D12" s="75"/>
+      <c r="E12" s="75"/>
+      <c r="F12" s="75"/>
+      <c r="G12" s="75"/>
+      <c r="H12" s="75"/>
       <c r="J12" s="59"/>
       <c r="K12" s="60"/>
-      <c r="L12" s="102"/>
+      <c r="L12" s="79"/>
       <c r="M12" s="48" t="s">
         <v>147</v>
       </c>
       <c r="N12" s="48" t="s">
         <v>147</v>
       </c>
-      <c r="O12" s="76"/>
+      <c r="O12" s="91"/>
       <c r="P12" s="48" t="s">
         <v>189</v>
       </c>
@@ -2248,27 +2251,29 @@
       </c>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B13" s="79" t="s">
+      <c r="B13" s="67" t="s">
         <v>151</v>
       </c>
-      <c r="C13" s="79"/>
-      <c r="D13" s="45"/>
+      <c r="C13" s="67"/>
+      <c r="D13" s="45" t="s">
+        <v>250</v>
+      </c>
       <c r="E13" s="45" t="s">
         <v>134</v>
       </c>
-      <c r="F13" s="87"/>
-      <c r="G13" s="87"/>
-      <c r="H13" s="87"/>
+      <c r="F13" s="73"/>
+      <c r="G13" s="73"/>
+      <c r="H13" s="73"/>
       <c r="J13" s="59"/>
       <c r="K13" s="60"/>
-      <c r="L13" s="102"/>
+      <c r="L13" s="79"/>
       <c r="M13" s="48" t="s">
         <v>19</v>
       </c>
       <c r="N13" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="O13" s="76"/>
+      <c r="O13" s="91"/>
       <c r="P13" s="53" t="s">
         <v>190</v>
       </c>
@@ -2277,27 +2282,27 @@
       </c>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B14" s="79" t="s">
+      <c r="B14" s="67" t="s">
         <v>154</v>
       </c>
-      <c r="C14" s="79"/>
+      <c r="C14" s="67"/>
       <c r="D14" s="45"/>
       <c r="E14" s="45" t="s">
         <v>134</v>
       </c>
-      <c r="F14" s="87"/>
-      <c r="G14" s="87"/>
-      <c r="H14" s="87"/>
+      <c r="F14" s="73"/>
+      <c r="G14" s="73"/>
+      <c r="H14" s="73"/>
       <c r="J14" s="61"/>
       <c r="K14" s="62"/>
-      <c r="L14" s="102"/>
+      <c r="L14" s="79"/>
       <c r="M14" s="48" t="s">
         <v>148</v>
       </c>
       <c r="N14" s="48" t="s">
         <v>148</v>
       </c>
-      <c r="O14" s="76"/>
+      <c r="O14" s="91"/>
       <c r="P14" s="53" t="s">
         <v>191</v>
       </c>
@@ -2306,29 +2311,29 @@
       </c>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B15" s="79" t="s">
+      <c r="B15" s="67" t="s">
         <v>155</v>
       </c>
-      <c r="C15" s="79"/>
+      <c r="C15" s="67"/>
       <c r="D15" s="45"/>
       <c r="E15" s="45" t="s">
         <v>134</v>
       </c>
-      <c r="F15" s="87"/>
-      <c r="G15" s="87"/>
-      <c r="H15" s="87"/>
-      <c r="J15" s="99" t="s">
+      <c r="F15" s="73"/>
+      <c r="G15" s="73"/>
+      <c r="H15" s="73"/>
+      <c r="J15" s="76" t="s">
         <v>104</v>
       </c>
-      <c r="K15" s="100"/>
-      <c r="L15" s="102"/>
+      <c r="K15" s="77"/>
+      <c r="L15" s="79"/>
       <c r="M15" s="48" t="s">
         <v>15</v>
       </c>
       <c r="N15" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="O15" s="76"/>
+      <c r="O15" s="91"/>
       <c r="P15" s="53" t="s">
         <v>192</v>
       </c>
@@ -2337,31 +2342,31 @@
       </c>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B16" s="79" t="s">
+      <c r="B16" s="67" t="s">
         <v>157</v>
       </c>
-      <c r="C16" s="79"/>
+      <c r="C16" s="67"/>
       <c r="D16" s="47"/>
       <c r="E16" s="51" t="s">
         <v>134</v>
       </c>
-      <c r="F16" s="87"/>
-      <c r="G16" s="87"/>
-      <c r="H16" s="87"/>
+      <c r="F16" s="73"/>
+      <c r="G16" s="73"/>
+      <c r="H16" s="73"/>
       <c r="J16" s="48" t="s">
         <v>105</v>
       </c>
       <c r="K16" s="48" t="s">
         <v>116</v>
       </c>
-      <c r="L16" s="102"/>
+      <c r="L16" s="79"/>
       <c r="M16" s="48" t="s">
         <v>149</v>
       </c>
       <c r="N16" s="48" t="s">
         <v>149</v>
       </c>
-      <c r="O16" s="76"/>
+      <c r="O16" s="91"/>
       <c r="P16" s="48" t="s">
         <v>197</v>
       </c>
@@ -2370,29 +2375,29 @@
       </c>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B17" s="79" t="s">
+      <c r="B17" s="67" t="s">
         <v>156</v>
       </c>
-      <c r="C17" s="79"/>
+      <c r="C17" s="67"/>
       <c r="D17" s="47"/>
       <c r="E17" s="51" t="s">
         <v>134</v>
       </c>
-      <c r="F17" s="87"/>
-      <c r="G17" s="87"/>
-      <c r="H17" s="87"/>
+      <c r="F17" s="73"/>
+      <c r="G17" s="73"/>
+      <c r="H17" s="73"/>
       <c r="J17" s="48" t="s">
         <v>0</v>
       </c>
       <c r="K17" s="48" t="s">
         <v>110</v>
       </c>
-      <c r="L17" s="102"/>
-      <c r="M17" s="99" t="s">
+      <c r="L17" s="79"/>
+      <c r="M17" s="76" t="s">
         <v>161</v>
       </c>
-      <c r="N17" s="100"/>
-      <c r="O17" s="76"/>
+      <c r="N17" s="77"/>
+      <c r="O17" s="91"/>
       <c r="P17" s="53" t="s">
         <v>198</v>
       </c>
@@ -2401,31 +2406,33 @@
       </c>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B18" s="77" t="s">
+      <c r="B18" s="92" t="s">
         <v>153</v>
       </c>
-      <c r="C18" s="78"/>
-      <c r="D18" s="47"/>
+      <c r="C18" s="93"/>
+      <c r="D18" s="47" t="s">
+        <v>250</v>
+      </c>
       <c r="E18" s="51" t="s">
         <v>134</v>
       </c>
-      <c r="F18" s="87"/>
-      <c r="G18" s="87"/>
-      <c r="H18" s="87"/>
+      <c r="F18" s="73"/>
+      <c r="G18" s="73"/>
+      <c r="H18" s="73"/>
       <c r="J18" s="48" t="s">
         <v>106</v>
       </c>
       <c r="K18" s="48" t="s">
         <v>111</v>
       </c>
-      <c r="L18" s="102"/>
+      <c r="L18" s="79"/>
       <c r="M18" s="56" t="s">
         <v>171</v>
       </c>
       <c r="N18" s="32" t="s">
         <v>143</v>
       </c>
-      <c r="O18" s="76"/>
+      <c r="O18" s="91"/>
       <c r="P18" s="53" t="s">
         <v>199</v>
       </c>
@@ -2434,31 +2441,31 @@
       </c>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B19" s="77" t="s">
+      <c r="B19" s="92" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="78"/>
+      <c r="C19" s="93"/>
       <c r="D19" s="47"/>
       <c r="E19" s="51" t="s">
         <v>134</v>
       </c>
-      <c r="F19" s="87"/>
-      <c r="G19" s="87"/>
-      <c r="H19" s="87"/>
+      <c r="F19" s="73"/>
+      <c r="G19" s="73"/>
+      <c r="H19" s="73"/>
       <c r="J19" s="48" t="s">
         <v>107</v>
       </c>
       <c r="K19" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="L19" s="102"/>
+      <c r="L19" s="79"/>
       <c r="M19" s="49" t="s">
         <v>162</v>
       </c>
       <c r="N19" s="49" t="s">
         <v>79</v>
       </c>
-      <c r="O19" s="76"/>
+      <c r="O19" s="91"/>
       <c r="P19" s="53" t="s">
         <v>200</v>
       </c>
@@ -2467,18 +2474,20 @@
       </c>
     </row>
     <row r="20" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="90" t="s">
+      <c r="B20" s="95" t="s">
         <v>152</v>
       </c>
-      <c r="C20" s="91"/>
-      <c r="D20" s="45"/>
-      <c r="E20" s="96" t="s">
+      <c r="C20" s="96"/>
+      <c r="D20" s="45">
+        <v>2</v>
+      </c>
+      <c r="E20" s="101" t="s">
         <v>158</v>
       </c>
-      <c r="F20" s="86" t="s">
+      <c r="F20" s="94" t="s">
         <v>159</v>
       </c>
-      <c r="G20" s="86"/>
+      <c r="G20" s="94"/>
       <c r="H20" s="52"/>
       <c r="J20" s="48" t="s">
         <v>113</v>
@@ -2486,14 +2495,14 @@
       <c r="K20" s="48" t="s">
         <v>117</v>
       </c>
-      <c r="L20" s="102"/>
+      <c r="L20" s="79"/>
       <c r="M20" s="49" t="s">
         <v>163</v>
       </c>
       <c r="N20" s="49" t="s">
         <v>80</v>
       </c>
-      <c r="O20" s="76"/>
+      <c r="O20" s="91"/>
       <c r="P20" s="48" t="s">
         <v>205</v>
       </c>
@@ -2502,12 +2511,12 @@
       </c>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B21" s="92"/>
-      <c r="C21" s="93"/>
+      <c r="B21" s="97"/>
+      <c r="C21" s="98"/>
       <c r="D21" s="45"/>
-      <c r="E21" s="97"/>
-      <c r="F21" s="86"/>
-      <c r="G21" s="86"/>
+      <c r="E21" s="102"/>
+      <c r="F21" s="94"/>
+      <c r="G21" s="94"/>
       <c r="H21" s="52"/>
       <c r="J21" s="48" t="s">
         <v>108</v>
@@ -2515,14 +2524,14 @@
       <c r="K21" s="48" t="s">
         <v>112</v>
       </c>
-      <c r="L21" s="102"/>
+      <c r="L21" s="79"/>
       <c r="M21" s="49" t="s">
         <v>164</v>
       </c>
       <c r="N21" s="49" t="s">
         <v>168</v>
       </c>
-      <c r="O21" s="76"/>
+      <c r="O21" s="91"/>
       <c r="P21" s="53" t="s">
         <v>206</v>
       </c>
@@ -2531,12 +2540,12 @@
       </c>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B22" s="92"/>
-      <c r="C22" s="93"/>
+      <c r="B22" s="97"/>
+      <c r="C22" s="98"/>
       <c r="D22" s="45"/>
-      <c r="E22" s="97"/>
-      <c r="F22" s="86"/>
-      <c r="G22" s="86"/>
+      <c r="E22" s="102"/>
+      <c r="F22" s="94"/>
+      <c r="G22" s="94"/>
       <c r="H22" s="52"/>
       <c r="J22" s="32" t="s">
         <v>119</v>
@@ -2544,14 +2553,14 @@
       <c r="K22" s="32" t="s">
         <v>120</v>
       </c>
-      <c r="L22" s="103"/>
+      <c r="L22" s="80"/>
       <c r="M22" s="49" t="s">
         <v>165</v>
       </c>
       <c r="N22" s="48" t="s">
         <v>167</v>
       </c>
-      <c r="O22" s="76"/>
+      <c r="O22" s="91"/>
       <c r="P22" s="53" t="s">
         <v>207</v>
       </c>
@@ -2560,19 +2569,19 @@
       </c>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B23" s="92"/>
-      <c r="C23" s="93"/>
+      <c r="B23" s="97"/>
+      <c r="C23" s="98"/>
       <c r="D23" s="45"/>
-      <c r="E23" s="97"/>
-      <c r="F23" s="86"/>
-      <c r="G23" s="86"/>
+      <c r="E23" s="102"/>
+      <c r="F23" s="94"/>
+      <c r="G23" s="94"/>
       <c r="H23" s="52"/>
-      <c r="J23" s="66"/>
-      <c r="K23" s="67"/>
-      <c r="L23" s="67"/>
-      <c r="M23" s="67"/>
-      <c r="N23" s="68"/>
-      <c r="O23" s="76"/>
+      <c r="J23" s="81"/>
+      <c r="K23" s="82"/>
+      <c r="L23" s="82"/>
+      <c r="M23" s="82"/>
+      <c r="N23" s="83"/>
+      <c r="O23" s="91"/>
       <c r="P23" s="53" t="s">
         <v>208</v>
       </c>
@@ -2581,19 +2590,19 @@
       </c>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B24" s="92"/>
-      <c r="C24" s="93"/>
+      <c r="B24" s="97"/>
+      <c r="C24" s="98"/>
       <c r="D24" s="45"/>
-      <c r="E24" s="97"/>
-      <c r="F24" s="86"/>
-      <c r="G24" s="86"/>
+      <c r="E24" s="102"/>
+      <c r="F24" s="94"/>
+      <c r="G24" s="94"/>
       <c r="H24" s="52"/>
-      <c r="J24" s="69"/>
-      <c r="K24" s="70"/>
-      <c r="L24" s="70"/>
-      <c r="M24" s="70"/>
-      <c r="N24" s="71"/>
-      <c r="O24" s="76"/>
+      <c r="J24" s="84"/>
+      <c r="K24" s="85"/>
+      <c r="L24" s="85"/>
+      <c r="M24" s="85"/>
+      <c r="N24" s="86"/>
+      <c r="O24" s="91"/>
       <c r="P24" s="32" t="s">
         <v>214</v>
       </c>
@@ -2602,19 +2611,19 @@
       </c>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B25" s="92"/>
-      <c r="C25" s="93"/>
+      <c r="B25" s="97"/>
+      <c r="C25" s="98"/>
       <c r="D25" s="45"/>
-      <c r="E25" s="97"/>
-      <c r="F25" s="86"/>
-      <c r="G25" s="86"/>
+      <c r="E25" s="102"/>
+      <c r="F25" s="94"/>
+      <c r="G25" s="94"/>
       <c r="H25" s="52"/>
-      <c r="J25" s="69"/>
-      <c r="K25" s="70"/>
-      <c r="L25" s="70"/>
-      <c r="M25" s="70"/>
-      <c r="N25" s="71"/>
-      <c r="O25" s="76"/>
+      <c r="J25" s="84"/>
+      <c r="K25" s="85"/>
+      <c r="L25" s="85"/>
+      <c r="M25" s="85"/>
+      <c r="N25" s="86"/>
+      <c r="O25" s="91"/>
       <c r="P25" s="32" t="s">
         <v>218</v>
       </c>
@@ -2623,19 +2632,19 @@
       </c>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B26" s="92"/>
-      <c r="C26" s="93"/>
+      <c r="B26" s="97"/>
+      <c r="C26" s="98"/>
       <c r="D26" s="45"/>
-      <c r="E26" s="97"/>
-      <c r="F26" s="86"/>
-      <c r="G26" s="86"/>
+      <c r="E26" s="102"/>
+      <c r="F26" s="94"/>
+      <c r="G26" s="94"/>
       <c r="H26" s="52"/>
-      <c r="J26" s="69"/>
-      <c r="K26" s="70"/>
-      <c r="L26" s="70"/>
-      <c r="M26" s="70"/>
-      <c r="N26" s="71"/>
-      <c r="O26" s="76"/>
+      <c r="J26" s="84"/>
+      <c r="K26" s="85"/>
+      <c r="L26" s="85"/>
+      <c r="M26" s="85"/>
+      <c r="N26" s="86"/>
+      <c r="O26" s="91"/>
       <c r="P26" s="32" t="s">
         <v>219</v>
       </c>
@@ -2644,19 +2653,19 @@
       </c>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B27" s="94"/>
-      <c r="C27" s="95"/>
+      <c r="B27" s="99"/>
+      <c r="C27" s="100"/>
       <c r="D27" s="45"/>
-      <c r="E27" s="98"/>
-      <c r="F27" s="86"/>
-      <c r="G27" s="86"/>
+      <c r="E27" s="103"/>
+      <c r="F27" s="94"/>
+      <c r="G27" s="94"/>
       <c r="H27" s="52"/>
-      <c r="J27" s="69"/>
-      <c r="K27" s="70"/>
-      <c r="L27" s="70"/>
-      <c r="M27" s="70"/>
-      <c r="N27" s="71"/>
-      <c r="O27" s="76"/>
+      <c r="J27" s="84"/>
+      <c r="K27" s="85"/>
+      <c r="L27" s="85"/>
+      <c r="M27" s="85"/>
+      <c r="N27" s="86"/>
+      <c r="O27" s="91"/>
       <c r="P27" s="32" t="s">
         <v>220</v>
       </c>
@@ -2665,12 +2674,12 @@
       </c>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="J28" s="69"/>
-      <c r="K28" s="70"/>
-      <c r="L28" s="70"/>
-      <c r="M28" s="70"/>
-      <c r="N28" s="71"/>
-      <c r="O28" s="76"/>
+      <c r="J28" s="84"/>
+      <c r="K28" s="85"/>
+      <c r="L28" s="85"/>
+      <c r="M28" s="85"/>
+      <c r="N28" s="86"/>
+      <c r="O28" s="91"/>
       <c r="P28" s="32" t="s">
         <v>222</v>
       </c>
@@ -2679,12 +2688,12 @@
       </c>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="J29" s="69"/>
-      <c r="K29" s="70"/>
-      <c r="L29" s="70"/>
-      <c r="M29" s="70"/>
-      <c r="N29" s="71"/>
-      <c r="O29" s="76"/>
+      <c r="J29" s="84"/>
+      <c r="K29" s="85"/>
+      <c r="L29" s="85"/>
+      <c r="M29" s="85"/>
+      <c r="N29" s="86"/>
+      <c r="O29" s="91"/>
       <c r="P29" s="32" t="s">
         <v>221</v>
       </c>
@@ -2693,12 +2702,12 @@
       </c>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="J30" s="69"/>
-      <c r="K30" s="70"/>
-      <c r="L30" s="70"/>
-      <c r="M30" s="70"/>
-      <c r="N30" s="71"/>
-      <c r="O30" s="76"/>
+      <c r="J30" s="84"/>
+      <c r="K30" s="85"/>
+      <c r="L30" s="85"/>
+      <c r="M30" s="85"/>
+      <c r="N30" s="86"/>
+      <c r="O30" s="91"/>
       <c r="P30" s="32" t="s">
         <v>223</v>
       </c>
@@ -2707,12 +2716,12 @@
       </c>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="J31" s="69"/>
-      <c r="K31" s="70"/>
-      <c r="L31" s="70"/>
-      <c r="M31" s="70"/>
-      <c r="N31" s="71"/>
-      <c r="O31" s="76"/>
+      <c r="J31" s="84"/>
+      <c r="K31" s="85"/>
+      <c r="L31" s="85"/>
+      <c r="M31" s="85"/>
+      <c r="N31" s="86"/>
+      <c r="O31" s="91"/>
       <c r="P31" s="32" t="s">
         <v>224</v>
       </c>
@@ -2721,12 +2730,12 @@
       </c>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="J32" s="69"/>
-      <c r="K32" s="70"/>
-      <c r="L32" s="70"/>
-      <c r="M32" s="70"/>
-      <c r="N32" s="71"/>
-      <c r="O32" s="76"/>
+      <c r="J32" s="84"/>
+      <c r="K32" s="85"/>
+      <c r="L32" s="85"/>
+      <c r="M32" s="85"/>
+      <c r="N32" s="86"/>
+      <c r="O32" s="91"/>
       <c r="P32" s="32" t="s">
         <v>225</v>
       </c>
@@ -2735,12 +2744,12 @@
       </c>
     </row>
     <row r="33" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J33" s="69"/>
-      <c r="K33" s="70"/>
-      <c r="L33" s="70"/>
-      <c r="M33" s="70"/>
-      <c r="N33" s="71"/>
-      <c r="O33" s="76"/>
+      <c r="J33" s="84"/>
+      <c r="K33" s="85"/>
+      <c r="L33" s="85"/>
+      <c r="M33" s="85"/>
+      <c r="N33" s="86"/>
+      <c r="O33" s="91"/>
       <c r="P33" s="32" t="s">
         <v>226</v>
       </c>
@@ -2749,12 +2758,12 @@
       </c>
     </row>
     <row r="34" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J34" s="69"/>
-      <c r="K34" s="70"/>
-      <c r="L34" s="70"/>
-      <c r="M34" s="70"/>
-      <c r="N34" s="71"/>
-      <c r="O34" s="76"/>
+      <c r="J34" s="84"/>
+      <c r="K34" s="85"/>
+      <c r="L34" s="85"/>
+      <c r="M34" s="85"/>
+      <c r="N34" s="86"/>
+      <c r="O34" s="91"/>
       <c r="P34" s="32" t="s">
         <v>227</v>
       </c>
@@ -2763,12 +2772,12 @@
       </c>
     </row>
     <row r="35" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J35" s="69"/>
-      <c r="K35" s="70"/>
-      <c r="L35" s="70"/>
-      <c r="M35" s="70"/>
-      <c r="N35" s="71"/>
-      <c r="O35" s="76"/>
+      <c r="J35" s="84"/>
+      <c r="K35" s="85"/>
+      <c r="L35" s="85"/>
+      <c r="M35" s="85"/>
+      <c r="N35" s="86"/>
+      <c r="O35" s="91"/>
       <c r="P35" s="32" t="s">
         <v>228</v>
       </c>
@@ -2777,12 +2786,12 @@
       </c>
     </row>
     <row r="36" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J36" s="69"/>
-      <c r="K36" s="70"/>
-      <c r="L36" s="70"/>
-      <c r="M36" s="70"/>
-      <c r="N36" s="71"/>
-      <c r="O36" s="76"/>
+      <c r="J36" s="84"/>
+      <c r="K36" s="85"/>
+      <c r="L36" s="85"/>
+      <c r="M36" s="85"/>
+      <c r="N36" s="86"/>
+      <c r="O36" s="91"/>
       <c r="P36" s="32" t="s">
         <v>237</v>
       </c>
@@ -2791,12 +2800,12 @@
       </c>
     </row>
     <row r="37" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J37" s="69"/>
-      <c r="K37" s="70"/>
-      <c r="L37" s="70"/>
-      <c r="M37" s="70"/>
-      <c r="N37" s="71"/>
-      <c r="O37" s="76"/>
+      <c r="J37" s="84"/>
+      <c r="K37" s="85"/>
+      <c r="L37" s="85"/>
+      <c r="M37" s="85"/>
+      <c r="N37" s="86"/>
+      <c r="O37" s="91"/>
       <c r="P37" s="32" t="s">
         <v>238</v>
       </c>
@@ -2805,12 +2814,12 @@
       </c>
     </row>
     <row r="38" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J38" s="72"/>
-      <c r="K38" s="73"/>
-      <c r="L38" s="73"/>
-      <c r="M38" s="73"/>
-      <c r="N38" s="74"/>
-      <c r="O38" s="76"/>
+      <c r="J38" s="87"/>
+      <c r="K38" s="88"/>
+      <c r="L38" s="88"/>
+      <c r="M38" s="88"/>
+      <c r="N38" s="89"/>
+      <c r="O38" s="91"/>
       <c r="P38" s="32" t="s">
         <v>239</v>
       </c>
@@ -2828,6 +2837,18 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="J23:N38"/>
+    <mergeCell ref="O3:O38"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="F20:G27"/>
+    <mergeCell ref="B20:C27"/>
+    <mergeCell ref="E20:E27"/>
+    <mergeCell ref="M3:N3"/>
     <mergeCell ref="J2:Q2"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B14:C14"/>
@@ -2844,18 +2865,6 @@
     <mergeCell ref="L3:L22"/>
     <mergeCell ref="J15:K15"/>
     <mergeCell ref="M17:N17"/>
-    <mergeCell ref="J23:N38"/>
-    <mergeCell ref="O3:O38"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="F20:G27"/>
-    <mergeCell ref="B20:C27"/>
-    <mergeCell ref="E20:E27"/>
-    <mergeCell ref="M3:N3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2887,118 +2896,118 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A1" s="87"/>
-      <c r="B1" s="87"/>
-      <c r="C1" s="79" t="s">
+      <c r="A1" s="73"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="67" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79" t="s">
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
-      <c r="K1" s="79"/>
-      <c r="L1" s="79" t="s">
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="67"/>
+      <c r="L1" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="79"/>
-      <c r="N1" s="79"/>
-      <c r="O1" s="79" t="s">
+      <c r="M1" s="67"/>
+      <c r="N1" s="67"/>
+      <c r="O1" s="67" t="s">
         <v>41</v>
       </c>
-      <c r="P1" s="79"/>
-      <c r="Q1" s="79"/>
-      <c r="R1" s="79"/>
-      <c r="S1" s="79" t="s">
+      <c r="P1" s="67"/>
+      <c r="Q1" s="67"/>
+      <c r="R1" s="67"/>
+      <c r="S1" s="67" t="s">
         <v>34</v>
       </c>
-      <c r="T1" s="79"/>
-      <c r="U1" s="79"/>
-      <c r="V1" s="79"/>
-      <c r="W1" s="79"/>
-      <c r="X1" s="79"/>
-      <c r="Y1" s="79"/>
-      <c r="Z1" s="79"/>
-      <c r="AA1" s="79"/>
-      <c r="AB1" s="79"/>
-      <c r="AC1" s="79"/>
-      <c r="AD1" s="79"/>
-      <c r="AE1" s="79"/>
-      <c r="AF1" s="79"/>
-      <c r="AG1" s="79"/>
-      <c r="AH1" s="79"/>
-      <c r="AI1" s="79"/>
-      <c r="AJ1" s="79"/>
-      <c r="AK1" s="79"/>
+      <c r="T1" s="67"/>
+      <c r="U1" s="67"/>
+      <c r="V1" s="67"/>
+      <c r="W1" s="67"/>
+      <c r="X1" s="67"/>
+      <c r="Y1" s="67"/>
+      <c r="Z1" s="67"/>
+      <c r="AA1" s="67"/>
+      <c r="AB1" s="67"/>
+      <c r="AC1" s="67"/>
+      <c r="AD1" s="67"/>
+      <c r="AE1" s="67"/>
+      <c r="AF1" s="67"/>
+      <c r="AG1" s="67"/>
+      <c r="AH1" s="67"/>
+      <c r="AI1" s="67"/>
+      <c r="AJ1" s="67"/>
+      <c r="AK1" s="67"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A2" s="87"/>
-      <c r="B2" s="87"/>
-      <c r="C2" s="106" t="s">
+      <c r="A2" s="73"/>
+      <c r="B2" s="73"/>
+      <c r="C2" s="105" t="s">
         <v>82</v>
       </c>
-      <c r="D2" s="106"/>
-      <c r="E2" s="106"/>
-      <c r="F2" s="106" t="s">
+      <c r="D2" s="105"/>
+      <c r="E2" s="105"/>
+      <c r="F2" s="105" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="106"/>
-      <c r="H2" s="106"/>
-      <c r="I2" s="106" t="s">
+      <c r="G2" s="105"/>
+      <c r="H2" s="105"/>
+      <c r="I2" s="105" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="106"/>
-      <c r="K2" s="106"/>
-      <c r="L2" s="79" t="s">
+      <c r="J2" s="105"/>
+      <c r="K2" s="105"/>
+      <c r="L2" s="67" t="s">
         <v>33</v>
       </c>
-      <c r="M2" s="79"/>
-      <c r="N2" s="79"/>
-      <c r="O2" s="79" t="s">
+      <c r="M2" s="67"/>
+      <c r="N2" s="67"/>
+      <c r="O2" s="67" t="s">
         <v>38</v>
       </c>
-      <c r="P2" s="79"/>
-      <c r="Q2" s="79"/>
-      <c r="R2" s="86" t="s">
+      <c r="P2" s="67"/>
+      <c r="Q2" s="67"/>
+      <c r="R2" s="94" t="s">
         <v>94</v>
       </c>
-      <c r="S2" s="105" t="s">
-        <v>0</v>
-      </c>
-      <c r="T2" s="106" t="s">
+      <c r="S2" s="104" t="s">
+        <v>0</v>
+      </c>
+      <c r="T2" s="105" t="s">
         <v>103</v>
       </c>
-      <c r="U2" s="106"/>
-      <c r="V2" s="106"/>
-      <c r="W2" s="79" t="s">
+      <c r="U2" s="105"/>
+      <c r="V2" s="105"/>
+      <c r="W2" s="67" t="s">
         <v>101</v>
       </c>
-      <c r="X2" s="79"/>
-      <c r="Y2" s="79"/>
-      <c r="Z2" s="77" t="s">
+      <c r="X2" s="67"/>
+      <c r="Y2" s="67"/>
+      <c r="Z2" s="92" t="s">
         <v>102</v>
       </c>
-      <c r="AA2" s="104"/>
-      <c r="AB2" s="78"/>
-      <c r="AC2" s="79" t="s">
+      <c r="AA2" s="106"/>
+      <c r="AB2" s="93"/>
+      <c r="AC2" s="67" t="s">
         <v>99</v>
       </c>
-      <c r="AD2" s="79"/>
-      <c r="AE2" s="79"/>
-      <c r="AF2" s="79" t="s">
+      <c r="AD2" s="67"/>
+      <c r="AE2" s="67"/>
+      <c r="AF2" s="67" t="s">
         <v>100</v>
       </c>
-      <c r="AG2" s="79"/>
-      <c r="AH2" s="79"/>
-      <c r="AI2" s="79" t="s">
+      <c r="AG2" s="67"/>
+      <c r="AH2" s="67"/>
+      <c r="AI2" s="67" t="s">
         <v>83</v>
       </c>
-      <c r="AJ2" s="79"/>
-      <c r="AK2" s="79"/>
+      <c r="AJ2" s="67"/>
+      <c r="AK2" s="67"/>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
@@ -3052,8 +3061,8 @@
       <c r="Q3" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="R3" s="86"/>
-      <c r="S3" s="105"/>
+      <c r="R3" s="94"/>
+      <c r="S3" s="104"/>
       <c r="T3" s="16" t="s">
         <v>69</v>
       </c>
@@ -6637,6 +6646,12 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="W2:Y2"/>
+    <mergeCell ref="AC2:AE2"/>
+    <mergeCell ref="AF2:AH2"/>
+    <mergeCell ref="AI2:AK2"/>
+    <mergeCell ref="S1:AK1"/>
+    <mergeCell ref="Z2:AB2"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="S2:S3"/>
     <mergeCell ref="T2:V2"/>
@@ -6650,12 +6665,6 @@
     <mergeCell ref="L2:N2"/>
     <mergeCell ref="L1:N1"/>
     <mergeCell ref="C1:E1"/>
-    <mergeCell ref="W2:Y2"/>
-    <mergeCell ref="AC2:AE2"/>
-    <mergeCell ref="AF2:AH2"/>
-    <mergeCell ref="AI2:AK2"/>
-    <mergeCell ref="S1:AK1"/>
-    <mergeCell ref="Z2:AB2"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -6687,16 +6696,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="108" t="s">
+      <c r="A1" s="107" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="108"/>
-      <c r="C1" s="108"/>
-      <c r="D1" s="108"/>
-      <c r="E1" s="108"/>
-      <c r="F1" s="108"/>
-      <c r="G1" s="108"/>
-      <c r="H1" s="108"/>
+      <c r="B1" s="107"/>
+      <c r="C1" s="107"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="107"/>
+      <c r="F1" s="107"/>
+      <c r="G1" s="107"/>
+      <c r="H1" s="107"/>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
@@ -6727,11 +6736,11 @@
       <c r="E2" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="109" t="s">
+      <c r="F2" s="108" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="109"/>
-      <c r="H2" s="109"/>
+      <c r="G2" s="108"/>
+      <c r="H2" s="108"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -6803,19 +6812,19 @@
       <c r="X4" s="10"/>
     </row>
     <row r="5" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="108" t="s">
+      <c r="A5" s="107" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="108"/>
-      <c r="C5" s="108"/>
-      <c r="D5" s="108"/>
-      <c r="E5" s="108"/>
-      <c r="F5" s="108"/>
-      <c r="G5" s="108"/>
-      <c r="H5" s="108"/>
-      <c r="I5" s="108"/>
-      <c r="J5" s="108"/>
-      <c r="K5" s="108"/>
+      <c r="B5" s="107"/>
+      <c r="C5" s="107"/>
+      <c r="D5" s="107"/>
+      <c r="E5" s="107"/>
+      <c r="F5" s="107"/>
+      <c r="G5" s="107"/>
+      <c r="H5" s="107"/>
+      <c r="I5" s="107"/>
+      <c r="J5" s="107"/>
+      <c r="K5" s="107"/>
       <c r="R5" s="10"/>
       <c r="S5" s="10"/>
       <c r="T5" s="10"/>
@@ -6840,16 +6849,16 @@
       <c r="E6" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="113" t="s">
+      <c r="F6" s="110" t="s">
         <v>53</v>
       </c>
-      <c r="G6" s="114"/>
-      <c r="H6" s="115"/>
-      <c r="I6" s="113" t="s">
+      <c r="G6" s="111"/>
+      <c r="H6" s="112"/>
+      <c r="I6" s="110" t="s">
         <v>54</v>
       </c>
-      <c r="J6" s="114"/>
-      <c r="K6" s="115"/>
+      <c r="J6" s="111"/>
+      <c r="K6" s="112"/>
       <c r="L6" s="20"/>
       <c r="M6" s="20"/>
       <c r="N6" s="20"/>
@@ -6885,22 +6894,22 @@
       <c r="X7" s="10"/>
     </row>
     <row r="8" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="108" t="s">
+      <c r="A8" s="107" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="108"/>
-      <c r="C8" s="108"/>
-      <c r="D8" s="108"/>
-      <c r="E8" s="108"/>
-      <c r="F8" s="108"/>
-      <c r="G8" s="108"/>
-      <c r="H8" s="108"/>
-      <c r="I8" s="108"/>
-      <c r="J8" s="108"/>
-      <c r="K8" s="108"/>
-      <c r="L8" s="108"/>
-      <c r="M8" s="108"/>
-      <c r="N8" s="108"/>
+      <c r="B8" s="107"/>
+      <c r="C8" s="107"/>
+      <c r="D8" s="107"/>
+      <c r="E8" s="107"/>
+      <c r="F8" s="107"/>
+      <c r="G8" s="107"/>
+      <c r="H8" s="107"/>
+      <c r="I8" s="107"/>
+      <c r="J8" s="107"/>
+      <c r="K8" s="107"/>
+      <c r="L8" s="107"/>
+      <c r="M8" s="107"/>
+      <c r="N8" s="107"/>
       <c r="R8" s="10"/>
       <c r="S8" s="10"/>
       <c r="T8" s="10"/>
@@ -6925,21 +6934,21 @@
       <c r="E9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="109" t="s">
+      <c r="F9" s="108" t="s">
         <v>47</v>
       </c>
-      <c r="G9" s="109"/>
-      <c r="H9" s="109"/>
-      <c r="I9" s="107" t="s">
+      <c r="G9" s="108"/>
+      <c r="H9" s="108"/>
+      <c r="I9" s="109" t="s">
         <v>48</v>
       </c>
-      <c r="J9" s="107"/>
-      <c r="K9" s="107"/>
-      <c r="L9" s="107" t="s">
+      <c r="J9" s="109"/>
+      <c r="K9" s="109"/>
+      <c r="L9" s="109" t="s">
         <v>49</v>
       </c>
-      <c r="M9" s="107"/>
-      <c r="N9" s="107"/>
+      <c r="M9" s="109"/>
+      <c r="N9" s="109"/>
       <c r="R9" s="10"/>
       <c r="S9" s="10"/>
       <c r="T9" s="10"/>
@@ -7021,19 +7030,19 @@
       <c r="X11" s="10"/>
     </row>
     <row r="12" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="108" t="s">
+      <c r="A12" s="107" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="108"/>
-      <c r="C12" s="108"/>
-      <c r="D12" s="108"/>
-      <c r="E12" s="108"/>
-      <c r="F12" s="108"/>
-      <c r="G12" s="108"/>
-      <c r="H12" s="108"/>
-      <c r="I12" s="108"/>
-      <c r="J12" s="108"/>
-      <c r="K12" s="108"/>
+      <c r="B12" s="107"/>
+      <c r="C12" s="107"/>
+      <c r="D12" s="107"/>
+      <c r="E12" s="107"/>
+      <c r="F12" s="107"/>
+      <c r="G12" s="107"/>
+      <c r="H12" s="107"/>
+      <c r="I12" s="107"/>
+      <c r="J12" s="107"/>
+      <c r="K12" s="107"/>
       <c r="R12" s="10"/>
       <c r="S12" s="10"/>
       <c r="T12" s="10"/>
@@ -7058,16 +7067,16 @@
       <c r="E13" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="109" t="s">
+      <c r="F13" s="108" t="s">
         <v>47</v>
       </c>
-      <c r="G13" s="109"/>
-      <c r="H13" s="109"/>
-      <c r="I13" s="107" t="s">
+      <c r="G13" s="108"/>
+      <c r="H13" s="108"/>
+      <c r="I13" s="109" t="s">
         <v>50</v>
       </c>
-      <c r="J13" s="107"/>
-      <c r="K13" s="107"/>
+      <c r="J13" s="109"/>
+      <c r="K13" s="109"/>
       <c r="R13" s="10"/>
       <c r="S13" s="10"/>
       <c r="T13" s="10"/>
@@ -7145,19 +7154,19 @@
       <c r="X16" s="10"/>
     </row>
     <row r="17" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A17" s="108" t="s">
+      <c r="A17" s="107" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="108"/>
-      <c r="C17" s="108"/>
-      <c r="D17" s="108"/>
-      <c r="E17" s="108"/>
-      <c r="F17" s="108"/>
-      <c r="G17" s="108"/>
-      <c r="H17" s="108"/>
-      <c r="I17" s="108"/>
-      <c r="J17" s="108"/>
-      <c r="K17" s="108"/>
+      <c r="B17" s="107"/>
+      <c r="C17" s="107"/>
+      <c r="D17" s="107"/>
+      <c r="E17" s="107"/>
+      <c r="F17" s="107"/>
+      <c r="G17" s="107"/>
+      <c r="H17" s="107"/>
+      <c r="I17" s="107"/>
+      <c r="J17" s="107"/>
+      <c r="K17" s="107"/>
       <c r="R17" s="10"/>
       <c r="S17" s="10"/>
       <c r="T17" s="10"/>
@@ -7182,16 +7191,16 @@
       <c r="E18" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F18" s="109" t="s">
+      <c r="F18" s="108" t="s">
         <v>47</v>
       </c>
-      <c r="G18" s="109"/>
-      <c r="H18" s="109"/>
-      <c r="I18" s="107" t="s">
+      <c r="G18" s="108"/>
+      <c r="H18" s="108"/>
+      <c r="I18" s="109" t="s">
         <v>48</v>
       </c>
-      <c r="J18" s="107"/>
-      <c r="K18" s="107"/>
+      <c r="J18" s="109"/>
+      <c r="K18" s="109"/>
     </row>
     <row r="19" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
@@ -7228,19 +7237,19 @@
       <c r="X20" s="10"/>
     </row>
     <row r="21" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A21" s="108" t="s">
+      <c r="A21" s="107" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="108"/>
-      <c r="C21" s="108"/>
-      <c r="D21" s="108"/>
-      <c r="E21" s="108"/>
-      <c r="F21" s="108"/>
-      <c r="G21" s="108"/>
-      <c r="H21" s="108"/>
-      <c r="I21" s="108"/>
-      <c r="J21" s="108"/>
-      <c r="K21" s="108"/>
+      <c r="B21" s="107"/>
+      <c r="C21" s="107"/>
+      <c r="D21" s="107"/>
+      <c r="E21" s="107"/>
+      <c r="F21" s="107"/>
+      <c r="G21" s="107"/>
+      <c r="H21" s="107"/>
+      <c r="I21" s="107"/>
+      <c r="J21" s="107"/>
+      <c r="K21" s="107"/>
       <c r="R21" s="10"/>
       <c r="S21" s="10"/>
       <c r="T21" s="10"/>
@@ -7265,16 +7274,16 @@
       <c r="E22" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F22" s="109" t="s">
+      <c r="F22" s="108" t="s">
         <v>47</v>
       </c>
-      <c r="G22" s="109"/>
-      <c r="H22" s="109"/>
-      <c r="I22" s="107" t="s">
+      <c r="G22" s="108"/>
+      <c r="H22" s="108"/>
+      <c r="I22" s="109" t="s">
         <v>11</v>
       </c>
-      <c r="J22" s="107"/>
-      <c r="K22" s="107"/>
+      <c r="J22" s="109"/>
+      <c r="K22" s="109"/>
     </row>
     <row r="23" spans="1:24" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="18">
@@ -7313,22 +7322,22 @@
     </row>
     <row r="24" spans="1:24" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:24" s="18" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A25" s="108" t="s">
+      <c r="A25" s="107" t="s">
         <v>135</v>
       </c>
-      <c r="B25" s="108"/>
-      <c r="C25" s="108"/>
-      <c r="D25" s="108"/>
-      <c r="E25" s="108"/>
-      <c r="F25" s="108"/>
-      <c r="G25" s="108"/>
-      <c r="H25" s="108"/>
-      <c r="I25" s="108"/>
-      <c r="J25" s="108"/>
-      <c r="K25" s="108"/>
-      <c r="L25" s="108"/>
-      <c r="M25" s="108"/>
-      <c r="N25" s="108"/>
+      <c r="B25" s="107"/>
+      <c r="C25" s="107"/>
+      <c r="D25" s="107"/>
+      <c r="E25" s="107"/>
+      <c r="F25" s="107"/>
+      <c r="G25" s="107"/>
+      <c r="H25" s="107"/>
+      <c r="I25" s="107"/>
+      <c r="J25" s="107"/>
+      <c r="K25" s="107"/>
+      <c r="L25" s="107"/>
+      <c r="M25" s="107"/>
+      <c r="N25" s="107"/>
     </row>
     <row r="26" spans="1:24" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="37" t="s">
@@ -7346,44 +7355,44 @@
       <c r="E26" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="F26" s="109" t="s">
+      <c r="F26" s="108" t="s">
         <v>53</v>
       </c>
-      <c r="G26" s="109"/>
-      <c r="H26" s="109"/>
-      <c r="I26" s="107" t="s">
+      <c r="G26" s="108"/>
+      <c r="H26" s="108"/>
+      <c r="I26" s="109" t="s">
         <v>54</v>
       </c>
-      <c r="J26" s="107"/>
-      <c r="K26" s="107"/>
-      <c r="L26" s="107" t="s">
+      <c r="J26" s="109"/>
+      <c r="K26" s="109"/>
+      <c r="L26" s="109" t="s">
         <v>136</v>
       </c>
-      <c r="M26" s="107"/>
-      <c r="N26" s="107"/>
+      <c r="M26" s="109"/>
+      <c r="N26" s="109"/>
     </row>
     <row r="27" spans="1:24" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="1:24" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="29" spans="1:24" s="18" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A29" s="108" t="s">
+      <c r="A29" s="107" t="s">
         <v>137</v>
       </c>
-      <c r="B29" s="108"/>
-      <c r="C29" s="108"/>
-      <c r="D29" s="108"/>
-      <c r="E29" s="108"/>
-      <c r="F29" s="108"/>
-      <c r="G29" s="108"/>
-      <c r="H29" s="108"/>
-      <c r="I29" s="108"/>
-      <c r="J29" s="108"/>
-      <c r="K29" s="108"/>
-      <c r="L29" s="108"/>
-      <c r="M29" s="108"/>
-      <c r="N29" s="108"/>
-      <c r="O29" s="108"/>
-      <c r="P29" s="108"/>
-      <c r="Q29" s="108"/>
+      <c r="B29" s="107"/>
+      <c r="C29" s="107"/>
+      <c r="D29" s="107"/>
+      <c r="E29" s="107"/>
+      <c r="F29" s="107"/>
+      <c r="G29" s="107"/>
+      <c r="H29" s="107"/>
+      <c r="I29" s="107"/>
+      <c r="J29" s="107"/>
+      <c r="K29" s="107"/>
+      <c r="L29" s="107"/>
+      <c r="M29" s="107"/>
+      <c r="N29" s="107"/>
+      <c r="O29" s="107"/>
+      <c r="P29" s="107"/>
+      <c r="Q29" s="107"/>
     </row>
     <row r="30" spans="1:24" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="37" t="s">
@@ -7401,26 +7410,26 @@
       <c r="E30" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="F30" s="113" t="s">
+      <c r="F30" s="110" t="s">
         <v>53</v>
       </c>
-      <c r="G30" s="114"/>
-      <c r="H30" s="115"/>
-      <c r="I30" s="113" t="s">
+      <c r="G30" s="111"/>
+      <c r="H30" s="112"/>
+      <c r="I30" s="110" t="s">
         <v>54</v>
       </c>
-      <c r="J30" s="114"/>
-      <c r="K30" s="115"/>
-      <c r="L30" s="107" t="s">
+      <c r="J30" s="111"/>
+      <c r="K30" s="112"/>
+      <c r="L30" s="109" t="s">
         <v>138</v>
       </c>
-      <c r="M30" s="107"/>
-      <c r="N30" s="107"/>
-      <c r="O30" s="107" t="s">
+      <c r="M30" s="109"/>
+      <c r="N30" s="109"/>
+      <c r="O30" s="109" t="s">
         <v>139</v>
       </c>
-      <c r="P30" s="107"/>
-      <c r="Q30" s="107"/>
+      <c r="P30" s="109"/>
+      <c r="Q30" s="109"/>
     </row>
     <row r="31" spans="1:24" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20"/>
@@ -7443,14 +7452,14 @@
     </row>
     <row r="32" spans="1:24" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A33" s="108" t="s">
+      <c r="A33" s="107" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="108"/>
-      <c r="C33" s="108"/>
-      <c r="D33" s="108"/>
-      <c r="E33" s="108"/>
-      <c r="F33" s="108"/>
+      <c r="B33" s="107"/>
+      <c r="C33" s="107"/>
+      <c r="D33" s="107"/>
+      <c r="E33" s="107"/>
+      <c r="F33" s="107"/>
       <c r="G33" s="11"/>
       <c r="H33" s="11"/>
       <c r="I33" s="11"/>
@@ -7524,12 +7533,12 @@
       <c r="X36" s="10"/>
     </row>
     <row r="37" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A37" s="108" t="s">
+      <c r="A37" s="107" t="s">
         <v>19</v>
       </c>
-      <c r="B37" s="108"/>
-      <c r="C37" s="108"/>
-      <c r="D37" s="108"/>
+      <c r="B37" s="107"/>
+      <c r="C37" s="107"/>
+      <c r="D37" s="107"/>
       <c r="E37" s="11"/>
       <c r="F37" s="11"/>
       <c r="G37" s="11"/>
@@ -7601,15 +7610,15 @@
       <c r="K40" s="11"/>
     </row>
     <row r="41" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A41" s="110" t="s">
+      <c r="A41" s="113" t="s">
         <v>20</v>
       </c>
-      <c r="B41" s="111"/>
-      <c r="C41" s="111"/>
-      <c r="D41" s="111"/>
-      <c r="E41" s="111"/>
-      <c r="F41" s="111"/>
-      <c r="G41" s="112"/>
+      <c r="B41" s="114"/>
+      <c r="C41" s="114"/>
+      <c r="D41" s="114"/>
+      <c r="E41" s="114"/>
+      <c r="F41" s="114"/>
+      <c r="G41" s="115"/>
       <c r="H41" s="12"/>
       <c r="I41" s="12"/>
       <c r="J41" s="10"/>
@@ -7629,11 +7638,11 @@
       <c r="D42" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E42" s="107" t="s">
+      <c r="E42" s="109" t="s">
         <v>21</v>
       </c>
-      <c r="F42" s="107"/>
-      <c r="G42" s="107"/>
+      <c r="F42" s="109"/>
+      <c r="G42" s="109"/>
       <c r="H42" s="12"/>
       <c r="I42" s="12"/>
       <c r="J42" s="10"/>
@@ -7757,21 +7766,6 @@
     <row r="64" spans="1:7" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="A8:N8"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="A5:K5"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="A12:K12"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="I13:K13"/>
-    <mergeCell ref="A17:K17"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="I18:K18"/>
     <mergeCell ref="E42:G42"/>
     <mergeCell ref="A21:K21"/>
     <mergeCell ref="F22:H22"/>
@@ -7788,6 +7782,21 @@
     <mergeCell ref="I30:K30"/>
     <mergeCell ref="L30:N30"/>
     <mergeCell ref="O30:Q30"/>
+    <mergeCell ref="A12:K12"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="I13:K13"/>
+    <mergeCell ref="A17:K17"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="A8:N8"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="A5:K5"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="I6:K6"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B20" xr:uid="{00000000-0002-0000-0100-000001000000}">
@@ -7926,56 +7935,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="122" t="s">
+      <c r="A1" s="123" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="123"/>
-      <c r="C1" s="123"/>
-      <c r="D1" s="123"/>
-      <c r="E1" s="123"/>
-      <c r="F1" s="123"/>
-      <c r="G1" s="123"/>
-      <c r="H1" s="123"/>
-      <c r="I1" s="123"/>
-      <c r="J1" s="123"/>
-      <c r="K1" s="123"/>
-      <c r="L1" s="123"/>
-      <c r="M1" s="123"/>
-      <c r="N1" s="123"/>
-      <c r="O1" s="123"/>
-      <c r="P1" s="123"/>
-      <c r="Q1" s="123"/>
-      <c r="R1" s="123"/>
+      <c r="B1" s="124"/>
+      <c r="C1" s="124"/>
+      <c r="D1" s="124"/>
+      <c r="E1" s="124"/>
+      <c r="F1" s="124"/>
+      <c r="G1" s="124"/>
+      <c r="H1" s="124"/>
+      <c r="I1" s="124"/>
+      <c r="J1" s="124"/>
+      <c r="K1" s="124"/>
+      <c r="L1" s="124"/>
+      <c r="M1" s="124"/>
+      <c r="N1" s="124"/>
+      <c r="O1" s="124"/>
+      <c r="P1" s="124"/>
+      <c r="Q1" s="124"/>
+      <c r="R1" s="124"/>
     </row>
     <row r="2" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="108"/>
-      <c r="B2" s="108"/>
-      <c r="C2" s="108"/>
-      <c r="D2" s="108"/>
-      <c r="E2" s="108"/>
-      <c r="F2" s="108"/>
-      <c r="G2" s="108"/>
-      <c r="H2" s="108"/>
-      <c r="I2" s="108"/>
-      <c r="J2" s="108"/>
-      <c r="K2" s="108"/>
-      <c r="L2" s="108"/>
-      <c r="M2" s="124" t="s">
+      <c r="A2" s="107"/>
+      <c r="B2" s="107"/>
+      <c r="C2" s="107"/>
+      <c r="D2" s="107"/>
+      <c r="E2" s="107"/>
+      <c r="F2" s="107"/>
+      <c r="G2" s="107"/>
+      <c r="H2" s="107"/>
+      <c r="I2" s="107"/>
+      <c r="J2" s="107"/>
+      <c r="K2" s="107"/>
+      <c r="L2" s="107"/>
+      <c r="M2" s="125" t="s">
         <v>124</v>
       </c>
-      <c r="N2" s="125"/>
-      <c r="O2" s="125"/>
-      <c r="P2" s="125"/>
-      <c r="Q2" s="125"/>
-      <c r="R2" s="126"/>
-      <c r="U2" s="127" t="s">
+      <c r="N2" s="126"/>
+      <c r="O2" s="126"/>
+      <c r="P2" s="126"/>
+      <c r="Q2" s="126"/>
+      <c r="R2" s="127"/>
+      <c r="U2" s="128" t="s">
         <v>132</v>
       </c>
-      <c r="V2" s="127"/>
-      <c r="W2" s="127"/>
-      <c r="X2" s="127"/>
-      <c r="Y2" s="127"/>
-      <c r="Z2" s="127"/>
+      <c r="V2" s="128"/>
+      <c r="W2" s="128"/>
+      <c r="X2" s="128"/>
+      <c r="Y2" s="128"/>
+      <c r="Z2" s="128"/>
     </row>
     <row r="3" spans="1:26" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="37" t="s">
@@ -7993,16 +8002,16 @@
       <c r="E3" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="128" t="s">
+      <c r="F3" s="129" t="s">
         <v>53</v>
       </c>
-      <c r="G3" s="129"/>
-      <c r="H3" s="130"/>
-      <c r="I3" s="131" t="s">
+      <c r="G3" s="130"/>
+      <c r="H3" s="131"/>
+      <c r="I3" s="121" t="s">
         <v>54</v>
       </c>
-      <c r="J3" s="131"/>
-      <c r="K3" s="131"/>
+      <c r="J3" s="121"/>
+      <c r="K3" s="121"/>
       <c r="L3" s="40" t="s">
         <v>122</v>
       </c>
@@ -8022,12 +8031,12 @@
         <v>131</v>
       </c>
       <c r="R3" s="132"/>
-      <c r="U3" s="127"/>
-      <c r="V3" s="127"/>
-      <c r="W3" s="127"/>
-      <c r="X3" s="127"/>
-      <c r="Y3" s="127"/>
-      <c r="Z3" s="127"/>
+      <c r="U3" s="128"/>
+      <c r="V3" s="128"/>
+      <c r="W3" s="128"/>
+      <c r="X3" s="128"/>
+      <c r="Y3" s="128"/>
+      <c r="Z3" s="128"/>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B4" s="44"/>
@@ -8046,71 +8055,71 @@
       <c r="O4" s="18"/>
       <c r="P4" s="18"/>
       <c r="Q4" s="18"/>
-      <c r="U4" s="127"/>
-      <c r="V4" s="127"/>
-      <c r="W4" s="127"/>
-      <c r="X4" s="127"/>
-      <c r="Y4" s="127"/>
-      <c r="Z4" s="127"/>
+      <c r="U4" s="128"/>
+      <c r="V4" s="128"/>
+      <c r="W4" s="128"/>
+      <c r="X4" s="128"/>
+      <c r="Y4" s="128"/>
+      <c r="Z4" s="128"/>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="L5" s="18"/>
-      <c r="U5" s="127"/>
-      <c r="V5" s="127"/>
-      <c r="W5" s="127"/>
-      <c r="X5" s="127"/>
-      <c r="Y5" s="127"/>
-      <c r="Z5" s="127"/>
+      <c r="U5" s="128"/>
+      <c r="V5" s="128"/>
+      <c r="W5" s="128"/>
+      <c r="X5" s="128"/>
+      <c r="Y5" s="128"/>
+      <c r="Z5" s="128"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="U6" s="127"/>
-      <c r="V6" s="127"/>
-      <c r="W6" s="127"/>
-      <c r="X6" s="127"/>
-      <c r="Y6" s="127"/>
-      <c r="Z6" s="127"/>
+      <c r="U6" s="128"/>
+      <c r="V6" s="128"/>
+      <c r="W6" s="128"/>
+      <c r="X6" s="128"/>
+      <c r="Y6" s="128"/>
+      <c r="Z6" s="128"/>
     </row>
     <row r="7" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="122" t="s">
+      <c r="A7" s="123" t="s">
         <v>80</v>
       </c>
-      <c r="B7" s="123"/>
-      <c r="C7" s="123"/>
-      <c r="D7" s="123"/>
-      <c r="E7" s="123"/>
-      <c r="F7" s="123"/>
-      <c r="G7" s="123"/>
-      <c r="H7" s="123"/>
-      <c r="I7" s="123"/>
-      <c r="J7" s="123"/>
-      <c r="K7" s="123"/>
-      <c r="L7" s="123"/>
-      <c r="M7" s="123"/>
-      <c r="N7" s="123"/>
-      <c r="O7" s="123"/>
-      <c r="P7" s="123"/>
-      <c r="Q7" s="123"/>
-      <c r="R7" s="123"/>
-      <c r="U7" s="127"/>
-      <c r="V7" s="127"/>
-      <c r="W7" s="127"/>
-      <c r="X7" s="127"/>
-      <c r="Y7" s="127"/>
-      <c r="Z7" s="127"/>
+      <c r="B7" s="124"/>
+      <c r="C7" s="124"/>
+      <c r="D7" s="124"/>
+      <c r="E7" s="124"/>
+      <c r="F7" s="124"/>
+      <c r="G7" s="124"/>
+      <c r="H7" s="124"/>
+      <c r="I7" s="124"/>
+      <c r="J7" s="124"/>
+      <c r="K7" s="124"/>
+      <c r="L7" s="124"/>
+      <c r="M7" s="124"/>
+      <c r="N7" s="124"/>
+      <c r="O7" s="124"/>
+      <c r="P7" s="124"/>
+      <c r="Q7" s="124"/>
+      <c r="R7" s="124"/>
+      <c r="U7" s="128"/>
+      <c r="V7" s="128"/>
+      <c r="W7" s="128"/>
+      <c r="X7" s="128"/>
+      <c r="Y7" s="128"/>
+      <c r="Z7" s="128"/>
     </row>
     <row r="8" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="108"/>
-      <c r="B8" s="108"/>
-      <c r="C8" s="108"/>
-      <c r="D8" s="108"/>
-      <c r="E8" s="108"/>
-      <c r="F8" s="108"/>
-      <c r="G8" s="108"/>
-      <c r="H8" s="108"/>
-      <c r="I8" s="108"/>
-      <c r="J8" s="108"/>
-      <c r="K8" s="108"/>
-      <c r="L8" s="108"/>
+      <c r="A8" s="107"/>
+      <c r="B8" s="107"/>
+      <c r="C8" s="107"/>
+      <c r="D8" s="107"/>
+      <c r="E8" s="107"/>
+      <c r="F8" s="107"/>
+      <c r="G8" s="107"/>
+      <c r="H8" s="107"/>
+      <c r="I8" s="107"/>
+      <c r="J8" s="107"/>
+      <c r="K8" s="107"/>
+      <c r="L8" s="107"/>
       <c r="M8" s="133" t="s">
         <v>128</v>
       </c>
@@ -8119,12 +8128,12 @@
       <c r="P8" s="134"/>
       <c r="Q8" s="134"/>
       <c r="R8" s="135"/>
-      <c r="U8" s="127"/>
-      <c r="V8" s="127"/>
-      <c r="W8" s="127"/>
-      <c r="X8" s="127"/>
-      <c r="Y8" s="127"/>
-      <c r="Z8" s="127"/>
+      <c r="U8" s="128"/>
+      <c r="V8" s="128"/>
+      <c r="W8" s="128"/>
+      <c r="X8" s="128"/>
+      <c r="Y8" s="128"/>
+      <c r="Z8" s="128"/>
     </row>
     <row r="9" spans="1:26" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="37" t="s">
@@ -8142,16 +8151,16 @@
       <c r="E9" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="128" t="s">
+      <c r="F9" s="129" t="s">
         <v>53</v>
       </c>
-      <c r="G9" s="129"/>
-      <c r="H9" s="130"/>
-      <c r="I9" s="131" t="s">
+      <c r="G9" s="130"/>
+      <c r="H9" s="131"/>
+      <c r="I9" s="121" t="s">
         <v>54</v>
       </c>
-      <c r="J9" s="131"/>
-      <c r="K9" s="131"/>
+      <c r="J9" s="121"/>
+      <c r="K9" s="121"/>
       <c r="L9" s="40" t="s">
         <v>123</v>
       </c>
@@ -8167,16 +8176,16 @@
       <c r="P9" s="43" t="s">
         <v>129</v>
       </c>
-      <c r="Q9" s="128" t="s">
+      <c r="Q9" s="129" t="s">
         <v>130</v>
       </c>
-      <c r="R9" s="130"/>
-      <c r="U9" s="127"/>
-      <c r="V9" s="127"/>
-      <c r="W9" s="127"/>
-      <c r="X9" s="127"/>
-      <c r="Y9" s="127"/>
-      <c r="Z9" s="127"/>
+      <c r="R9" s="131"/>
+      <c r="U9" s="128"/>
+      <c r="V9" s="128"/>
+      <c r="W9" s="128"/>
+      <c r="X9" s="128"/>
+      <c r="Y9" s="128"/>
+      <c r="Z9" s="128"/>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="38"/>
@@ -8192,12 +8201,12 @@
       <c r="K10" s="44"/>
       <c r="L10" s="44"/>
       <c r="M10" s="26"/>
-      <c r="U10" s="127"/>
-      <c r="V10" s="127"/>
-      <c r="W10" s="127"/>
-      <c r="X10" s="127"/>
-      <c r="Y10" s="127"/>
-      <c r="Z10" s="127"/>
+      <c r="U10" s="128"/>
+      <c r="V10" s="128"/>
+      <c r="W10" s="128"/>
+      <c r="X10" s="128"/>
+      <c r="Y10" s="128"/>
+      <c r="Z10" s="128"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="38"/>
@@ -8212,49 +8221,49 @@
       <c r="J11" s="38"/>
       <c r="K11" s="38"/>
       <c r="L11" s="38"/>
-      <c r="U11" s="127"/>
-      <c r="V11" s="127"/>
-      <c r="W11" s="127"/>
-      <c r="X11" s="127"/>
-      <c r="Y11" s="127"/>
-      <c r="Z11" s="127"/>
+      <c r="U11" s="128"/>
+      <c r="V11" s="128"/>
+      <c r="W11" s="128"/>
+      <c r="X11" s="128"/>
+      <c r="Y11" s="128"/>
+      <c r="Z11" s="128"/>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="U12" s="127"/>
-      <c r="V12" s="127"/>
-      <c r="W12" s="127"/>
-      <c r="X12" s="127"/>
-      <c r="Y12" s="127"/>
-      <c r="Z12" s="127"/>
+      <c r="U12" s="128"/>
+      <c r="V12" s="128"/>
+      <c r="W12" s="128"/>
+      <c r="X12" s="128"/>
+      <c r="Y12" s="128"/>
+      <c r="Z12" s="128"/>
     </row>
     <row r="13" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="110" t="s">
+      <c r="A13" s="113" t="s">
         <v>85</v>
       </c>
-      <c r="B13" s="111"/>
-      <c r="C13" s="111"/>
-      <c r="D13" s="111"/>
-      <c r="E13" s="111"/>
-      <c r="F13" s="111"/>
-      <c r="G13" s="111"/>
-      <c r="H13" s="111"/>
-      <c r="I13" s="111"/>
-      <c r="J13" s="111"/>
-      <c r="K13" s="111"/>
-      <c r="L13" s="111"/>
-      <c r="M13" s="111"/>
-      <c r="N13" s="111"/>
-      <c r="O13" s="111"/>
-      <c r="P13" s="111"/>
+      <c r="B13" s="114"/>
+      <c r="C13" s="114"/>
+      <c r="D13" s="114"/>
+      <c r="E13" s="114"/>
+      <c r="F13" s="114"/>
+      <c r="G13" s="114"/>
+      <c r="H13" s="114"/>
+      <c r="I13" s="114"/>
+      <c r="J13" s="114"/>
+      <c r="K13" s="114"/>
+      <c r="L13" s="114"/>
+      <c r="M13" s="114"/>
+      <c r="N13" s="114"/>
+      <c r="O13" s="114"/>
+      <c r="P13" s="114"/>
       <c r="Q13" s="35"/>
       <c r="R13" s="35"/>
       <c r="S13" s="35"/>
-      <c r="U13" s="127"/>
-      <c r="V13" s="127"/>
-      <c r="W13" s="127"/>
-      <c r="X13" s="127"/>
-      <c r="Y13" s="127"/>
-      <c r="Z13" s="127"/>
+      <c r="U13" s="128"/>
+      <c r="V13" s="128"/>
+      <c r="W13" s="128"/>
+      <c r="X13" s="128"/>
+      <c r="Y13" s="128"/>
+      <c r="Z13" s="128"/>
     </row>
     <row r="14" spans="1:26" s="35" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="34" t="s">
@@ -8272,24 +8281,24 @@
       <c r="E14" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="F14" s="131" t="s">
+      <c r="F14" s="121" t="s">
         <v>90</v>
       </c>
-      <c r="G14" s="131"/>
-      <c r="H14" s="131"/>
+      <c r="G14" s="121"/>
+      <c r="H14" s="121"/>
       <c r="I14" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="J14" s="121" t="s">
+      <c r="J14" s="122" t="s">
         <v>11</v>
       </c>
-      <c r="K14" s="121"/>
-      <c r="L14" s="121"/>
-      <c r="M14" s="121" t="s">
+      <c r="K14" s="122"/>
+      <c r="L14" s="122"/>
+      <c r="M14" s="122" t="s">
         <v>84</v>
       </c>
-      <c r="N14" s="121"/>
-      <c r="O14" s="121"/>
+      <c r="N14" s="122"/>
+      <c r="O14" s="122"/>
       <c r="P14" s="36" t="s">
         <v>86</v>
       </c>
@@ -8337,20 +8346,20 @@
       <c r="S16" s="38"/>
     </row>
     <row r="17" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A17" s="110" t="s">
+      <c r="A17" s="113" t="s">
         <v>160</v>
       </c>
-      <c r="B17" s="111"/>
-      <c r="C17" s="111"/>
-      <c r="D17" s="111"/>
-      <c r="E17" s="111"/>
-      <c r="F17" s="111"/>
-      <c r="G17" s="111"/>
-      <c r="H17" s="111"/>
-      <c r="I17" s="111"/>
-      <c r="J17" s="111"/>
-      <c r="K17" s="111"/>
-      <c r="L17" s="111"/>
+      <c r="B17" s="114"/>
+      <c r="C17" s="114"/>
+      <c r="D17" s="114"/>
+      <c r="E17" s="114"/>
+      <c r="F17" s="114"/>
+      <c r="G17" s="114"/>
+      <c r="H17" s="114"/>
+      <c r="I17" s="114"/>
+      <c r="J17" s="114"/>
+      <c r="K17" s="114"/>
+      <c r="L17" s="114"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="48" t="s">
@@ -8368,16 +8377,16 @@
       <c r="E18" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="F18" s="79" t="s">
+      <c r="F18" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="G18" s="79"/>
-      <c r="H18" s="79"/>
-      <c r="I18" s="79" t="s">
+      <c r="G18" s="67"/>
+      <c r="H18" s="67"/>
+      <c r="I18" s="67" t="s">
         <v>169</v>
       </c>
-      <c r="J18" s="79"/>
-      <c r="K18" s="79"/>
+      <c r="J18" s="67"/>
+      <c r="K18" s="67"/>
       <c r="L18" s="33" t="s">
         <v>170</v>
       </c>
@@ -8426,11 +8435,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="A17:L17"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="J14:L14"/>
     <mergeCell ref="M14:O14"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="A2:L2"/>
@@ -8446,6 +8450,11 @@
     <mergeCell ref="I9:K9"/>
     <mergeCell ref="Q9:R9"/>
     <mergeCell ref="A13:P13"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="A17:L17"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="J14:L14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8455,7 +8464,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01937180-03B7-42C6-AC1A-CA356BC8C70D}">
   <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
@@ -8468,21 +8477,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="108" t="s">
+      <c r="A1" s="107" t="s">
         <v>245</v>
       </c>
-      <c r="B1" s="108"/>
-      <c r="C1" s="108"/>
-      <c r="F1" s="83" t="s">
+      <c r="B1" s="107"/>
+      <c r="C1" s="107"/>
+      <c r="F1" s="70" t="s">
         <v>166</v>
       </c>
-      <c r="G1" s="85"/>
-      <c r="I1" s="83" t="s">
+      <c r="G1" s="72"/>
+      <c r="I1" s="70" t="s">
         <v>249</v>
       </c>
-      <c r="J1" s="84"/>
-      <c r="K1" s="84"/>
-      <c r="L1" s="85"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="71"/>
+      <c r="L1" s="72"/>
     </row>
     <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="63" t="s">
@@ -8500,12 +8509,12 @@
       <c r="G2" s="63" t="s">
         <v>143</v>
       </c>
-      <c r="I2" s="127" t="s">
+      <c r="I2" s="128" t="s">
         <v>248</v>
       </c>
-      <c r="J2" s="127"/>
-      <c r="K2" s="127"/>
-      <c r="L2" s="127"/>
+      <c r="J2" s="128"/>
+      <c r="K2" s="128"/>
+      <c r="L2" s="128"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="63"/>
@@ -8517,10 +8526,10 @@
       <c r="G3" s="64" t="s">
         <v>175</v>
       </c>
-      <c r="I3" s="127"/>
-      <c r="J3" s="127"/>
-      <c r="K3" s="127"/>
-      <c r="L3" s="127"/>
+      <c r="I3" s="128"/>
+      <c r="J3" s="128"/>
+      <c r="K3" s="128"/>
+      <c r="L3" s="128"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="63"/>
@@ -8532,10 +8541,10 @@
       <c r="G4" s="64" t="s">
         <v>176</v>
       </c>
-      <c r="I4" s="127"/>
-      <c r="J4" s="127"/>
-      <c r="K4" s="127"/>
-      <c r="L4" s="127"/>
+      <c r="I4" s="128"/>
+      <c r="J4" s="128"/>
+      <c r="K4" s="128"/>
+      <c r="L4" s="128"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="63"/>
@@ -8547,10 +8556,10 @@
       <c r="G5" s="64" t="s">
         <v>179</v>
       </c>
-      <c r="I5" s="127"/>
-      <c r="J5" s="127"/>
-      <c r="K5" s="127"/>
-      <c r="L5" s="127"/>
+      <c r="I5" s="128"/>
+      <c r="J5" s="128"/>
+      <c r="K5" s="128"/>
+      <c r="L5" s="128"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="63"/>
@@ -8562,10 +8571,10 @@
       <c r="G6" s="64" t="s">
         <v>180</v>
       </c>
-      <c r="I6" s="127"/>
-      <c r="J6" s="127"/>
-      <c r="K6" s="127"/>
-      <c r="L6" s="127"/>
+      <c r="I6" s="128"/>
+      <c r="J6" s="128"/>
+      <c r="K6" s="128"/>
+      <c r="L6" s="128"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="63"/>

</xml_diff>